<commit_message>
New Projects Folders added
</commit_message>
<xml_diff>
--- a/Hardware Inteconnects.xlsx
+++ b/Hardware Inteconnects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kashif\OneDrive - Airzai\Airzai\GitHub\Airzai-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{048A1014-549B-439F-ABEF-BD58AA5E6648}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{86EE5462-6C3B-4C54-B680-B171D18F200B}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{048A1014-549B-439F-ABEF-BD58AA5E6648}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{D31B345C-234B-447B-80DC-CF0A0FE84F6E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BDE72F7E-F162-48FD-B3AC-A08C53C45481}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{BDE72F7E-F162-48FD-B3AC-A08C53C45481}"/>
   </bookViews>
   <sheets>
     <sheet name="Airzai Interconnects" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="49">
-  <si>
-    <t>Main Board J14</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="51">
   <si>
     <t>Pin Number</t>
   </si>
@@ -45,12 +42,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>LID Board</t>
-  </si>
-  <si>
-    <t>Flex Board</t>
-  </si>
-  <si>
     <t>J14</t>
   </si>
   <si>
@@ -178,6 +169,21 @@
   </si>
   <si>
     <t>J3</t>
+  </si>
+  <si>
+    <t>New Placement</t>
+  </si>
+  <si>
+    <t>LID Board Old Connections</t>
+  </si>
+  <si>
+    <t>Main Board J14 New Connections</t>
+  </si>
+  <si>
+    <t>Flex Board Old Connections</t>
+  </si>
+  <si>
+    <t>NFC Flex Board</t>
   </si>
 </sst>
 </file>
@@ -200,7 +206,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,6 +246,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -302,6 +314,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -320,10 +345,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC17FFE-34FD-4EEC-ACA2-98BFA418FDBF}">
-  <dimension ref="C2:R31"/>
+  <dimension ref="C2:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,653 +677,830 @@
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="3"/>
+    <row r="2" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="2"/>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-    </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="N6" s="3"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+    </row>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J7" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="K7" t="s">
         <v>10</v>
       </c>
       <c r="L7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" t="s">
         <v>1</v>
       </c>
-      <c r="M7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="Q7" t="s">
+        <v>0</v>
+      </c>
+      <c r="R7" t="s">
+        <v>10</v>
+      </c>
+      <c r="S7" t="s">
         <v>2</v>
       </c>
-      <c r="O7" t="s">
-        <v>1</v>
-      </c>
-      <c r="P7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q7" t="s">
+      <c r="T7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C8" s="7" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
-        <v>6</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="G8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="1">
         <v>20</v>
       </c>
-      <c r="J8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="L8" s="1">
+      <c r="K8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M8" s="1">
         <v>1</v>
       </c>
-      <c r="M8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="N8" t="s">
-        <v>9</v>
-      </c>
-      <c r="O8" s="1">
+      <c r="N8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="O8" s="8"/>
+      <c r="P8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="1">
         <v>1</v>
       </c>
-      <c r="P8" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="R8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="S8" s="8"/>
+      <c r="T8" s="1">
+        <v>1</v>
+      </c>
+      <c r="U8" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="G9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="J9" s="1">
         <v>19</v>
       </c>
-      <c r="J9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="1">
+      <c r="K9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="1">
         <v>2</v>
       </c>
-      <c r="M9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O9" s="1">
+      <c r="N9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" s="8"/>
+      <c r="Q9" s="1">
         <v>2</v>
       </c>
-      <c r="P9" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="R9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="S9" s="8"/>
+      <c r="T9" s="1">
+        <v>2</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="1">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="1">
         <v>18</v>
       </c>
-      <c r="J10" t="s">
-        <v>45</v>
-      </c>
-      <c r="L10" s="1">
+      <c r="K10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="1">
         <v>3</v>
       </c>
-      <c r="M10" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10" s="1">
+      <c r="N10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q10" s="1">
         <v>3</v>
       </c>
-      <c r="P10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="R10" t="s">
+        <v>16</v>
+      </c>
+      <c r="T10" s="1">
+        <v>3</v>
+      </c>
+      <c r="U10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D11" s="1">
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="1">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="1">
         <v>17</v>
       </c>
-      <c r="J11" t="s">
-        <v>46</v>
-      </c>
-      <c r="L11" s="1">
+      <c r="K11" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="1">
         <v>4</v>
       </c>
-      <c r="M11" t="s">
-        <v>20</v>
-      </c>
-      <c r="O11" s="1">
+      <c r="N11" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q11" s="1">
         <v>4</v>
       </c>
-      <c r="P11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="R11" t="s">
+        <v>17</v>
+      </c>
+      <c r="T11" s="1">
+        <v>4</v>
+      </c>
+      <c r="U11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D12" s="1">
         <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="1">
+        <v>12</v>
+      </c>
+      <c r="J12" s="1">
         <v>16</v>
       </c>
-      <c r="J12" t="s">
-        <v>47</v>
-      </c>
-      <c r="L12" s="1">
+      <c r="K12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M12" s="1">
         <v>5</v>
       </c>
-      <c r="M12" t="s">
-        <v>22</v>
-      </c>
-      <c r="O12" s="1">
+      <c r="N12" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="1">
         <v>5</v>
       </c>
-      <c r="P12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="R12" t="s">
+        <v>19</v>
+      </c>
+      <c r="T12" s="1">
+        <v>5</v>
+      </c>
+      <c r="U12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D13" s="1">
         <v>6</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="1">
+        <v>13</v>
+      </c>
+      <c r="J13" s="1">
         <v>15</v>
       </c>
-      <c r="J13" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" s="1">
+      <c r="K13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" s="1">
         <v>6</v>
       </c>
-      <c r="M13" t="s">
-        <v>23</v>
-      </c>
-      <c r="O13" s="1">
+      <c r="N13" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="1">
         <v>6</v>
       </c>
-      <c r="P13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="R13" t="s">
+        <v>20</v>
+      </c>
+      <c r="T13" s="1">
+        <v>6</v>
+      </c>
+      <c r="U13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D14" s="1">
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="1">
         <v>14</v>
       </c>
-      <c r="J14" t="s">
-        <v>12</v>
-      </c>
-      <c r="L14" s="1">
+      <c r="J14" s="1">
+        <v>14</v>
+      </c>
+      <c r="K14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="1">
         <v>7</v>
       </c>
-      <c r="M14" t="s">
-        <v>24</v>
-      </c>
-      <c r="O14" s="1">
+      <c r="N14" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" s="1">
         <v>7</v>
       </c>
-      <c r="P14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="R14" t="s">
+        <v>21</v>
+      </c>
+      <c r="T14" s="1">
+        <v>7</v>
+      </c>
+      <c r="U14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D15" s="1">
         <v>8</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="1">
+        <v>15</v>
+      </c>
+      <c r="J15" s="1">
         <v>13</v>
       </c>
-      <c r="J15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="1">
+      <c r="K15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="1">
         <v>8</v>
       </c>
-      <c r="O15" s="1">
+      <c r="Q15" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T15" s="1">
+        <v>8</v>
+      </c>
+      <c r="U15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D16" s="1">
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="1">
+        <v>16</v>
+      </c>
+      <c r="J16" s="1">
         <v>12</v>
       </c>
-      <c r="J16" t="s">
-        <v>19</v>
-      </c>
-      <c r="L16" s="1">
+      <c r="K16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M16" s="1">
         <v>9</v>
       </c>
-      <c r="M16" t="s">
-        <v>27</v>
-      </c>
-      <c r="O16" s="1">
+      <c r="N16" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q16" s="1">
         <v>9</v>
       </c>
-      <c r="P16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="R16" t="s">
+        <v>24</v>
+      </c>
+      <c r="T16" s="1">
+        <v>9</v>
+      </c>
+      <c r="U16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D17" s="1">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="1">
+        <v>17</v>
+      </c>
+      <c r="J17" s="1">
         <v>11</v>
       </c>
-      <c r="J17" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="1">
+      <c r="K17" t="s">
+        <v>17</v>
+      </c>
+      <c r="M17" s="1">
         <v>10</v>
       </c>
-      <c r="M17" t="s">
-        <v>26</v>
-      </c>
-      <c r="O17" s="1">
+      <c r="N17" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q17" s="1">
         <v>10</v>
       </c>
-      <c r="P17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="R17" t="s">
+        <v>23</v>
+      </c>
+      <c r="T17" s="1">
+        <v>10</v>
+      </c>
+      <c r="U17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="1">
+        <v>19</v>
+      </c>
+      <c r="J18" s="1">
         <v>10</v>
       </c>
-      <c r="J18" t="s">
-        <v>22</v>
-      </c>
-      <c r="L18" s="1">
+      <c r="K18" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="1">
         <v>11</v>
       </c>
-      <c r="M18" t="s">
-        <v>28</v>
-      </c>
-      <c r="O18" s="1">
+      <c r="N18" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="O18" s="17"/>
+      <c r="Q18" s="1">
         <v>11</v>
       </c>
-      <c r="P18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="R18" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="S18" s="17"/>
+      <c r="T18" s="1">
+        <v>11</v>
+      </c>
+      <c r="U18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <v>12</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I19" s="1">
+        <v>20</v>
+      </c>
+      <c r="J19" s="1">
         <v>9</v>
       </c>
-      <c r="J19" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" s="1">
+      <c r="K19" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="1">
         <v>12</v>
       </c>
-      <c r="M19" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="O19" s="1">
+      <c r="N19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="O19" s="9"/>
+      <c r="Q19" s="1">
         <v>12</v>
       </c>
-      <c r="P19" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="R19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="S19" s="9"/>
+      <c r="T19" s="1">
+        <v>12</v>
+      </c>
+      <c r="U19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20" s="1">
+        <v>21</v>
+      </c>
+      <c r="J20" s="1">
         <v>8</v>
       </c>
-      <c r="J20" t="s">
-        <v>24</v>
-      </c>
-      <c r="O20" s="1">
+      <c r="K20" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q20" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="T20" s="1">
+        <v>13</v>
+      </c>
+      <c r="U20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21" s="1">
+        <v>22</v>
+      </c>
+      <c r="J21" s="1">
         <v>7</v>
       </c>
-      <c r="J21" t="s">
-        <v>25</v>
-      </c>
-      <c r="O21" s="1">
+      <c r="K21" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q21" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="T21" s="1">
+        <v>14</v>
+      </c>
+      <c r="U21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <v>15</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" t="s">
-        <v>26</v>
-      </c>
-      <c r="I22" s="1">
+        <v>23</v>
+      </c>
+      <c r="H22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="1">
         <v>6</v>
       </c>
-      <c r="J22" t="s">
-        <v>26</v>
-      </c>
-      <c r="O22" s="1">
+      <c r="K22" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q22" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="T22" s="1">
+        <v>15</v>
+      </c>
+      <c r="U22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I23" s="1">
+        <v>24</v>
+      </c>
+      <c r="H23" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" s="1">
         <v>5</v>
       </c>
-      <c r="J23" t="s">
-        <v>27</v>
-      </c>
-      <c r="O23" s="1">
+      <c r="K23" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q23" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="T23" s="1">
+        <v>16</v>
+      </c>
+      <c r="U23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D24" s="1">
         <v>17</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" t="s">
-        <v>20</v>
-      </c>
-      <c r="I24" s="1">
+        <v>17</v>
+      </c>
+      <c r="J24" s="1">
         <v>4</v>
       </c>
-      <c r="J24" t="s">
-        <v>20</v>
-      </c>
-      <c r="O24" s="1">
+      <c r="K24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="Q24" s="1">
+        <v>17</v>
+      </c>
+      <c r="T24" s="1">
+        <v>17</v>
+      </c>
+      <c r="U24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D25" s="1">
         <v>18</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="1">
+      <c r="G25" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="17"/>
+      <c r="J25" s="1">
         <v>3</v>
       </c>
-      <c r="J25" t="s">
-        <v>28</v>
-      </c>
-      <c r="O25" s="1">
+      <c r="K25" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q25" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="T25" s="1">
+        <v>18</v>
+      </c>
+      <c r="U25" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D26" s="1">
         <v>19</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="I26" s="1">
+      <c r="G26" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="9"/>
+      <c r="J26" s="1">
         <v>2</v>
       </c>
-      <c r="J26" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="O26" s="1">
+      <c r="K26" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="Q26" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="T26" s="1">
+        <v>19</v>
+      </c>
+      <c r="U26" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
         <v>20</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="I27" s="1">
+      <c r="G27" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" s="9"/>
+      <c r="J27" s="1">
         <v>1</v>
       </c>
-      <c r="J27" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="O27" s="1">
+      <c r="K27" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="Q27" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-    </row>
-    <row r="29" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-    </row>
-    <row r="31" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="E31" s="13"/>
+      <c r="T27" s="1">
+        <v>20</v>
+      </c>
+      <c r="U27" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="U28" s="1"/>
+    </row>
+    <row r="29" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+    </row>
+    <row r="31" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E31" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C3:Q3"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="C3:T3"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="T6:V6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated interconnect details. May 8, 2019
</commit_message>
<xml_diff>
--- a/Hardware Inteconnects.xlsx
+++ b/Hardware Inteconnects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kashif\OneDrive - Airzai\Airzai\GitHub\Airzai-Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://teamairzai-my.sharepoint.com/personal/kashif_airzai_com/Documents/Airzai/GitHub/PCB Design/Airzai-PCB-Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="8_{048A1014-549B-439F-ABEF-BD58AA5E6648}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{D31B345C-234B-447B-80DC-CF0A0FE84F6E}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="6_{9706E25E-717C-4DF6-87EF-534170850AE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{646A1624-4FEF-4865-8A08-A39DEB635739}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{BDE72F7E-F162-48FD-B3AC-A08C53C45481}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BDE72F7E-F162-48FD-B3AC-A08C53C45481}"/>
   </bookViews>
   <sheets>
     <sheet name="Airzai Interconnects" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="68">
   <si>
     <t>Pin Number</t>
   </si>
@@ -48,9 +48,6 @@
     <t>J4</t>
   </si>
   <si>
-    <t>Airzai Board Interconnects Rev 1.0</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -180,10 +177,64 @@
     <t>Main Board J14 New Connections</t>
   </si>
   <si>
-    <t>Flex Board Old Connections</t>
-  </si>
-  <si>
     <t>NFC Flex Board</t>
+  </si>
+  <si>
+    <t>Airzai Board Interconnects Rev 2.0</t>
+  </si>
+  <si>
+    <t>Flex Board New Connections</t>
+  </si>
+  <si>
+    <t>Cap1 Touch Out</t>
+  </si>
+  <si>
+    <t>Cap2 Touch Out</t>
+  </si>
+  <si>
+    <t>Not needed</t>
+  </si>
+  <si>
+    <t>DNC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Name Old </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Name New </t>
+  </si>
+  <si>
+    <t>Hookup to NTC</t>
+  </si>
+  <si>
+    <t>Spare GPIO</t>
+  </si>
+  <si>
+    <t>To Turn ON/OFF Circuit</t>
+  </si>
+  <si>
+    <t>LED Str CLK</t>
+  </si>
+  <si>
+    <t>LED Str DATA</t>
+  </si>
+  <si>
+    <t>Hookup to Accelerometer</t>
+  </si>
+  <si>
+    <t>Connect to different GPIO Pin</t>
+  </si>
+  <si>
+    <t>P53_GPIO_30</t>
+  </si>
+  <si>
+    <t>Accel INT</t>
+  </si>
+  <si>
+    <t>Pull Up</t>
+  </si>
+  <si>
+    <t>NFC INT</t>
   </si>
 </sst>
 </file>
@@ -206,7 +257,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,6 +303,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -327,6 +396,18 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -342,10 +423,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -663,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC17FFE-34FD-4EEC-ACA2-98BFA418FDBF}">
-  <dimension ref="C2:V31"/>
+  <dimension ref="C2:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,133 +752,150 @@
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" customWidth="1"/>
     <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="11.5703125" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="2"/>
-    </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C6" s="11" t="s">
+    <row r="2" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="2"/>
+    </row>
+    <row r="6" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="C6" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-    </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
+    </row>
+    <row r="7" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7" t="s">
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J7" t="s">
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="L7" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="M7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" t="s">
         <v>0</v>
       </c>
-      <c r="N7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" t="s">
         <v>2</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R7" t="s">
         <v>1</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="S7" t="s">
         <v>0</v>
       </c>
-      <c r="R7" t="s">
-        <v>10</v>
-      </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
+        <v>9</v>
+      </c>
+      <c r="U7" t="s">
         <v>2</v>
       </c>
-      <c r="T7" t="s">
+      <c r="V7" t="s">
         <v>0</v>
       </c>
-      <c r="U7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="W7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
@@ -811,7 +905,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="7" t="s">
@@ -821,686 +915,795 @@
         <v>20</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="M8" s="1">
+        <v>7</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O8" s="1">
         <v>1</v>
       </c>
-      <c r="N8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="O8" s="8"/>
-      <c r="P8" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q8" s="1">
+      <c r="P8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q8" s="8"/>
+      <c r="R8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S8" s="1">
         <v>1</v>
       </c>
-      <c r="R8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="S8" s="8"/>
-      <c r="T8" s="1">
+      <c r="T8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="U8" s="8"/>
+      <c r="V8" s="1">
         <v>1</v>
       </c>
-      <c r="U8" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="W8" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H9" s="8"/>
       <c r="J9" s="1">
         <v>19</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="M9" s="1">
+        <v>7</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="O9" s="1">
         <v>2</v>
       </c>
-      <c r="N9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="O9" s="8"/>
-      <c r="Q9" s="1">
+      <c r="P9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="8"/>
+      <c r="S9" s="1">
         <v>2</v>
       </c>
-      <c r="R9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="S9" s="8"/>
-      <c r="T9" s="1">
+      <c r="T9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="U9" s="8"/>
+      <c r="V9" s="1">
         <v>2</v>
       </c>
-      <c r="U9" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="W9" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" t="s">
-        <v>9</v>
+      <c r="G10" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J10" s="1">
         <v>18</v>
       </c>
       <c r="K10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M10" s="1">
+        <v>41</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O10" s="1">
         <v>3</v>
       </c>
-      <c r="N10" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q10" s="1">
+      <c r="P10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>54</v>
+      </c>
+      <c r="S10" s="1">
         <v>3</v>
       </c>
-      <c r="R10" t="s">
-        <v>16</v>
-      </c>
-      <c r="T10" s="1">
+      <c r="T10" t="s">
+        <v>15</v>
+      </c>
+      <c r="U10" t="s">
+        <v>66</v>
+      </c>
+      <c r="V10" s="1">
         <v>3</v>
       </c>
-      <c r="U10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="W10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D11" s="1">
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" t="s">
-        <v>11</v>
+      <c r="G11" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J11" s="1">
         <v>17</v>
       </c>
       <c r="K11" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="1">
+        <v>42</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="1">
         <v>4</v>
       </c>
-      <c r="N11" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q11" s="1">
+      <c r="P11" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>54</v>
+      </c>
+      <c r="S11" s="1">
         <v>4</v>
       </c>
-      <c r="R11" t="s">
-        <v>17</v>
-      </c>
-      <c r="T11" s="1">
+      <c r="T11" t="s">
+        <v>16</v>
+      </c>
+      <c r="V11" s="1">
         <v>4</v>
       </c>
-      <c r="U11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="W11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D12" s="1">
         <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" t="s">
-        <v>12</v>
+      <c r="G12" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="J12" s="1">
         <v>16</v>
       </c>
       <c r="K12" t="s">
-        <v>44</v>
-      </c>
-      <c r="M12" s="1">
+        <v>43</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" t="s">
+        <v>57</v>
+      </c>
+      <c r="O12" s="1">
         <v>5</v>
       </c>
-      <c r="N12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q12" s="1">
+      <c r="P12" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>54</v>
+      </c>
+      <c r="S12" s="1">
         <v>5</v>
       </c>
-      <c r="R12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T12" s="1">
+      <c r="T12" t="s">
+        <v>18</v>
+      </c>
+      <c r="U12" t="s">
+        <v>53</v>
+      </c>
+      <c r="V12" s="1">
         <v>5</v>
       </c>
-      <c r="U12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="W12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D13" s="1">
         <v>6</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J13" s="1">
         <v>15</v>
       </c>
       <c r="K13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" t="s">
         <v>13</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" t="s">
+        <v>58</v>
+      </c>
+      <c r="O13" s="1">
         <v>6</v>
       </c>
-      <c r="N13" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q13" s="1">
+      <c r="P13" t="s">
+        <v>51</v>
+      </c>
+      <c r="S13" s="1">
         <v>6</v>
       </c>
-      <c r="R13" t="s">
-        <v>20</v>
-      </c>
-      <c r="T13" s="1">
+      <c r="T13" t="s">
+        <v>51</v>
+      </c>
+      <c r="V13" s="1">
         <v>6</v>
       </c>
-      <c r="U13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="W13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D14" s="1">
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" t="s">
-        <v>14</v>
+      <c r="G14" s="18" t="s">
+        <v>13</v>
       </c>
       <c r="J14" s="1">
         <v>14</v>
       </c>
       <c r="K14" t="s">
-        <v>9</v>
-      </c>
-      <c r="M14" s="1">
+        <v>8</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="O14" s="1">
         <v>7</v>
       </c>
-      <c r="N14" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q14" s="1">
+      <c r="P14" t="s">
+        <v>20</v>
+      </c>
+      <c r="S14" s="1">
         <v>7</v>
       </c>
-      <c r="R14" t="s">
-        <v>21</v>
-      </c>
-      <c r="T14" s="1">
+      <c r="T14" t="s">
+        <v>20</v>
+      </c>
+      <c r="V14" s="1">
         <v>7</v>
       </c>
-      <c r="U14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="W14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D15" s="1">
         <v>8</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" t="s">
-        <v>15</v>
+      <c r="G15" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="J15" s="1">
         <v>13</v>
       </c>
       <c r="K15" t="s">
-        <v>11</v>
-      </c>
-      <c r="M15" s="1">
+        <v>10</v>
+      </c>
+      <c r="L15" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="O15" s="1">
         <v>8</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="P15" t="s">
+        <v>52</v>
+      </c>
+      <c r="S15" s="1">
         <v>8</v>
       </c>
-      <c r="T15" s="1">
+      <c r="T15" t="s">
+        <v>52</v>
+      </c>
+      <c r="V15" s="1">
         <v>8</v>
       </c>
-      <c r="U15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="W15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D16" s="1">
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J16" s="1">
         <v>12</v>
       </c>
       <c r="K16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M16" s="1">
+        <v>15</v>
+      </c>
+      <c r="L16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" t="s">
+        <v>58</v>
+      </c>
+      <c r="O16" s="1">
         <v>9</v>
       </c>
-      <c r="N16" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q16" s="1">
+      <c r="P16" t="s">
+        <v>23</v>
+      </c>
+      <c r="S16" s="1">
         <v>9</v>
       </c>
-      <c r="R16" t="s">
-        <v>24</v>
-      </c>
-      <c r="T16" s="1">
+      <c r="T16" t="s">
+        <v>23</v>
+      </c>
+      <c r="V16" s="1">
         <v>9</v>
       </c>
-      <c r="U16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="W16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D17" s="1">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" t="s">
-        <v>17</v>
+      <c r="G17" s="16" t="s">
+        <v>60</v>
       </c>
       <c r="J17" s="1">
         <v>11</v>
       </c>
       <c r="K17" t="s">
-        <v>17</v>
-      </c>
-      <c r="M17" s="1">
+        <v>16</v>
+      </c>
+      <c r="L17" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="O17" s="1">
         <v>10</v>
       </c>
-      <c r="N17" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q17" s="1">
+      <c r="P17" t="s">
+        <v>22</v>
+      </c>
+      <c r="S17" s="1">
         <v>10</v>
       </c>
-      <c r="R17" t="s">
-        <v>23</v>
-      </c>
-      <c r="T17" s="1">
+      <c r="T17" t="s">
+        <v>22</v>
+      </c>
+      <c r="V17" s="1">
         <v>10</v>
       </c>
-      <c r="U17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="W17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="G18" t="s">
-        <v>19</v>
+      <c r="G18" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="J18" s="1">
         <v>10</v>
       </c>
       <c r="K18" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18" s="1">
+        <v>18</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="O18" s="1">
         <v>11</v>
       </c>
-      <c r="N18" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="O18" s="17"/>
-      <c r="Q18" s="1">
+      <c r="P18" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q18" s="12"/>
+      <c r="S18" s="1">
         <v>11</v>
       </c>
-      <c r="R18" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="S18" s="17"/>
-      <c r="T18" s="1">
+      <c r="T18" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="U18" s="12"/>
+      <c r="V18" s="1">
         <v>11</v>
       </c>
-      <c r="U18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="W18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <v>12</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="J19" s="1">
         <v>9</v>
       </c>
       <c r="K19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M19" s="1">
+        <v>19</v>
+      </c>
+      <c r="L19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M19" t="s">
+        <v>58</v>
+      </c>
+      <c r="O19" s="1">
         <v>12</v>
       </c>
-      <c r="N19" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="O19" s="9"/>
-      <c r="Q19" s="1">
+      <c r="P19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q19" s="9"/>
+      <c r="S19" s="1">
         <v>12</v>
       </c>
-      <c r="R19" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="S19" s="9"/>
-      <c r="T19" s="1">
+      <c r="T19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="U19" s="9"/>
+      <c r="V19" s="1">
         <v>12</v>
       </c>
-      <c r="U19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="W19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" t="s">
-        <v>21</v>
+      <c r="G20" s="17" t="s">
+        <v>20</v>
       </c>
       <c r="J20" s="1">
         <v>8</v>
       </c>
       <c r="K20" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q20" s="1">
+        <v>20</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="S20" s="1">
         <v>13</v>
       </c>
-      <c r="T20" s="1">
+      <c r="V20" s="1">
         <v>13</v>
       </c>
-      <c r="U20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="W20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F21" s="1"/>
-      <c r="G21" t="s">
-        <v>22</v>
+      <c r="G21" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" t="s">
+        <v>45</v>
       </c>
       <c r="J21" s="1">
         <v>7</v>
       </c>
       <c r="K21" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q21" s="1">
+        <v>21</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="M21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S21" s="1">
         <v>14</v>
       </c>
-      <c r="T21" s="1">
+      <c r="V21" s="1">
         <v>14</v>
       </c>
-      <c r="U21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="W21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <v>15</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" t="s">
-        <v>23</v>
+      <c r="G22" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="H22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J22" s="1">
         <v>6</v>
       </c>
-      <c r="K22" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q22" s="1">
+      <c r="K22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="S22" s="1">
         <v>15</v>
       </c>
-      <c r="T22" s="1">
+      <c r="V22" s="1">
         <v>15</v>
       </c>
-      <c r="U22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="W22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23" t="s">
-        <v>24</v>
+      <c r="G23" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="H23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J23" s="1">
         <v>5</v>
       </c>
-      <c r="K23" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q23" s="1">
+      <c r="K23" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L23" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="S23" s="1">
         <v>16</v>
       </c>
-      <c r="T23" s="1">
+      <c r="V23" s="1">
         <v>16</v>
       </c>
-      <c r="U23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="W23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D24" s="1">
         <v>17</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="1"/>
+      <c r="E24" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J24" s="1">
         <v>4</v>
       </c>
       <c r="K24" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" t="s">
+        <v>16</v>
+      </c>
+      <c r="M24" t="s">
+        <v>59</v>
+      </c>
+      <c r="S24" s="1">
         <v>17</v>
       </c>
-      <c r="Q24" s="1">
+      <c r="V24" s="1">
         <v>17</v>
       </c>
-      <c r="T24" s="1">
-        <v>17</v>
-      </c>
-      <c r="U24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="W24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D25" s="1">
         <v>18</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H25" s="17"/>
+      <c r="G25" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="12"/>
       <c r="J25" s="1">
         <v>3</v>
       </c>
-      <c r="K25" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q25" s="1">
+      <c r="K25" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="S25" s="1">
         <v>18</v>
       </c>
-      <c r="T25" s="1">
+      <c r="V25" s="1">
         <v>18</v>
       </c>
-      <c r="U25" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="W25" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D26" s="1">
         <v>19</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H26" s="9"/>
       <c r="J26" s="1">
         <v>2</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L26" s="10"/>
+        <v>25</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
-      <c r="Q26" s="1">
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="S26" s="1">
         <v>19</v>
       </c>
-      <c r="T26" s="1">
+      <c r="V26" s="1">
         <v>19</v>
       </c>
-      <c r="U26" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="W26" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
         <v>20</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H27" s="9"/>
       <c r="J27" s="1">
         <v>1</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L27" s="10"/>
+        <v>25</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
-      <c r="Q27" s="1">
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="S27" s="1">
         <v>20</v>
       </c>
-      <c r="T27" s="1">
+      <c r="V27" s="1">
         <v>20</v>
       </c>
-      <c r="U27" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="L28" s="10"/>
+      <c r="W27" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="4:23" x14ac:dyDescent="0.25">
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
-      <c r="U28" s="1"/>
-    </row>
-    <row r="29" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="L29" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="W28" s="1"/>
+    </row>
+    <row r="29" spans="4:23" x14ac:dyDescent="0.25">
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
-    </row>
-    <row r="31" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+    </row>
+    <row r="31" spans="4:23" x14ac:dyDescent="0.25">
       <c r="E31" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C3:T3"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="T6:V6"/>
+    <mergeCell ref="C3:V3"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="V6:X6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bom and Interconnect details updated
</commit_message>
<xml_diff>
--- a/Hardware Inteconnects.xlsx
+++ b/Hardware Inteconnects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://teamairzai-my.sharepoint.com/personal/kashif_airzai_com/Documents/Airzai/GitHub/PCB Design/Airzai-PCB-Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kashi\OneDrive - Airzai\Airzai\GitHub\PCB Design\Airzai-PCB-Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="6_{9706E25E-717C-4DF6-87EF-534170850AE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{646A1624-4FEF-4865-8A08-A39DEB635739}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="6_{9706E25E-717C-4DF6-87EF-534170850AE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{BD6E8713-6316-4695-91AC-E575F64590AD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BDE72F7E-F162-48FD-B3AC-A08C53C45481}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="30915" windowHeight="15796" xr2:uid="{BDE72F7E-F162-48FD-B3AC-A08C53C45481}"/>
   </bookViews>
   <sheets>
     <sheet name="Airzai Interconnects" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="69">
   <si>
     <t>Pin Number</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>NFC INT</t>
+  </si>
+  <si>
+    <t>SW1 GPIO</t>
   </si>
 </sst>
 </file>
@@ -742,38 +745,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC17FFE-34FD-4EEC-ACA2-98BFA418FDBF}">
   <dimension ref="C2:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" customWidth="1"/>
-    <col min="13" max="13" width="27.7109375" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" customWidth="1"/>
-    <col min="18" max="18" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" customWidth="1"/>
-    <col min="21" max="21" width="11.5703125" customWidth="1"/>
-    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.59765625" customWidth="1"/>
+    <col min="9" max="9" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.59765625" customWidth="1"/>
+    <col min="12" max="12" width="21.86328125" customWidth="1"/>
+    <col min="13" max="13" width="27.73046875" customWidth="1"/>
+    <col min="14" max="14" width="21.73046875" customWidth="1"/>
+    <col min="15" max="15" width="11.59765625" customWidth="1"/>
+    <col min="16" max="16" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.73046875" customWidth="1"/>
+    <col min="18" max="18" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.73046875" customWidth="1"/>
+    <col min="21" max="21" width="11.59765625" customWidth="1"/>
+    <col min="22" max="22" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:24" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="3:24" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C3" s="20" t="s">
         <v>49</v>
       </c>
@@ -798,7 +801,7 @@
       <c r="V3" s="22"/>
       <c r="W3" s="2"/>
     </row>
-    <row r="6" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:24" x14ac:dyDescent="0.45">
       <c r="C6" s="19" t="s">
         <v>47</v>
       </c>
@@ -830,7 +833,7 @@
       <c r="W6" s="24"/>
       <c r="X6" s="24"/>
     </row>
-    <row r="7" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:24" x14ac:dyDescent="0.45">
       <c r="C7" t="s">
         <v>6</v>
       </c>
@@ -895,7 +898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:24" x14ac:dyDescent="0.45">
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
@@ -948,7 +951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:24" x14ac:dyDescent="0.45">
       <c r="D9" s="1">
         <v>2</v>
       </c>
@@ -988,7 +991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:24" x14ac:dyDescent="0.45">
       <c r="D10" s="1">
         <v>3</v>
       </c>
@@ -1036,7 +1039,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:24" x14ac:dyDescent="0.45">
       <c r="D11" s="1">
         <v>4</v>
       </c>
@@ -1081,7 +1084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:24" x14ac:dyDescent="0.45">
       <c r="D12" s="1">
         <v>5</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:24" x14ac:dyDescent="0.45">
       <c r="D13" s="1">
         <v>6</v>
       </c>
@@ -1171,7 +1174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:24" x14ac:dyDescent="0.45">
       <c r="D14" s="1">
         <v>7</v>
       </c>
@@ -1210,7 +1213,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:24" x14ac:dyDescent="0.45">
       <c r="D15" s="1">
         <v>8</v>
       </c>
@@ -1249,7 +1252,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:24" x14ac:dyDescent="0.45">
       <c r="D16" s="1">
         <v>9</v>
       </c>
@@ -1267,10 +1270,10 @@
         <v>15</v>
       </c>
       <c r="L16" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="M16" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="O16" s="1">
         <v>9</v>
@@ -1291,7 +1294,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:23" x14ac:dyDescent="0.45">
       <c r="D17" s="1">
         <v>10</v>
       </c>
@@ -1330,7 +1333,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:23" x14ac:dyDescent="0.45">
       <c r="D18" s="1">
         <v>11</v>
       </c>
@@ -1371,7 +1374,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:23" x14ac:dyDescent="0.45">
       <c r="D19" s="1">
         <v>12</v>
       </c>
@@ -1415,7 +1418,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:23" x14ac:dyDescent="0.45">
       <c r="D20" s="1">
         <v>13</v>
       </c>
@@ -1445,7 +1448,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:23" x14ac:dyDescent="0.45">
       <c r="D21" s="1">
         <v>14</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:23" x14ac:dyDescent="0.45">
       <c r="D22" s="1">
         <v>15</v>
       </c>
@@ -1514,7 +1517,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:23" x14ac:dyDescent="0.45">
       <c r="D23" s="1">
         <v>16</v>
       </c>
@@ -1547,7 +1550,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:23" x14ac:dyDescent="0.45">
       <c r="D24" s="1">
         <v>17</v>
       </c>
@@ -1582,7 +1585,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:23" x14ac:dyDescent="0.45">
       <c r="D25" s="1">
         <v>18</v>
       </c>
@@ -1611,7 +1614,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:23" x14ac:dyDescent="0.45">
       <c r="D26" s="1">
         <v>19</v>
       </c>
@@ -1645,7 +1648,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:23" x14ac:dyDescent="0.45">
       <c r="D27" s="1">
         <v>20</v>
       </c>
@@ -1679,7 +1682,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:23" x14ac:dyDescent="0.45">
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
@@ -1687,14 +1690,14 @@
       <c r="Q28" s="10"/>
       <c r="W28" s="1"/>
     </row>
-    <row r="29" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:23" x14ac:dyDescent="0.45">
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
     </row>
-    <row r="31" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:23" x14ac:dyDescent="0.45">
       <c r="E31" s="10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in schematics and BOM
</commit_message>
<xml_diff>
--- a/Hardware Inteconnects.xlsx
+++ b/Hardware Inteconnects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kashif\OneDrive - Airzai\Airzai\GitHub\Airzai-Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajeeth\OneDrive\Weekly updates\GitHub\Airzai-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{048A1014-549B-439F-ABEF-BD58AA5E6648}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{86EE5462-6C3B-4C54-B680-B171D18F200B}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="6_{9706E25E-717C-4DF6-87EF-534170850AE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{9B874EAD-C379-49FB-BF3A-549A32E0A229}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BDE72F7E-F162-48FD-B3AC-A08C53C45481}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="49">
-  <si>
-    <t>Main Board J14</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="71">
   <si>
     <t>Pin Number</t>
   </si>
@@ -45,21 +42,12 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>LID Board</t>
-  </si>
-  <si>
-    <t>Flex Board</t>
-  </si>
-  <si>
     <t>J14</t>
   </si>
   <si>
     <t>J4</t>
   </si>
   <si>
-    <t>Airzai Board Interconnects Rev 1.0</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -178,6 +166,84 @@
   </si>
   <si>
     <t>J3</t>
+  </si>
+  <si>
+    <t>New Placement</t>
+  </si>
+  <si>
+    <t>LID Board Old Connections</t>
+  </si>
+  <si>
+    <t>Main Board J14 New Connections</t>
+  </si>
+  <si>
+    <t>NFC Flex Board</t>
+  </si>
+  <si>
+    <t>Airzai Board Interconnects Rev 2.0</t>
+  </si>
+  <si>
+    <t>Flex Board New Connections</t>
+  </si>
+  <si>
+    <t>Cap1 Touch Out</t>
+  </si>
+  <si>
+    <t>Cap2 Touch Out</t>
+  </si>
+  <si>
+    <t>Not needed</t>
+  </si>
+  <si>
+    <t>DNC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Name Old </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Name New </t>
+  </si>
+  <si>
+    <t>Hookup to NTC</t>
+  </si>
+  <si>
+    <t>Spare GPIO</t>
+  </si>
+  <si>
+    <t>To Turn ON/OFF Circuit</t>
+  </si>
+  <si>
+    <t>LED Str CLK</t>
+  </si>
+  <si>
+    <t>LED Str DATA</t>
+  </si>
+  <si>
+    <t>Hookup to Accelerometer</t>
+  </si>
+  <si>
+    <t>Connect to different GPIO Pin</t>
+  </si>
+  <si>
+    <t>P53_GPIO_30</t>
+  </si>
+  <si>
+    <t>Accel INT</t>
+  </si>
+  <si>
+    <t>Pull Up</t>
+  </si>
+  <si>
+    <t>NFC INT</t>
+  </si>
+  <si>
+    <t>Atomizer 2</t>
+  </si>
+  <si>
+    <t>Atomizer 1</t>
+  </si>
+  <si>
+    <t>TOF sensor</t>
   </si>
 </sst>
 </file>
@@ -200,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,6 +306,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -302,6 +392,31 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -317,13 +432,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC17FFE-34FD-4EEC-ACA2-98BFA418FDBF}">
-  <dimension ref="C2:R31"/>
+  <dimension ref="C2:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView tabSelected="1" topLeftCell="I6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,655 +761,967 @@
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
+    <row r="2" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="2"/>
+    </row>
+    <row r="6" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="C6" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
+    </row>
+    <row r="7" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-    </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" t="s">
+        <v>56</v>
+      </c>
+      <c r="M7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="S7" t="s">
+        <v>0</v>
+      </c>
+      <c r="T7" t="s">
+        <v>9</v>
+      </c>
+      <c r="U7" t="s">
         <v>2</v>
       </c>
-      <c r="O7" t="s">
-        <v>1</v>
-      </c>
-      <c r="P7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q7" t="s">
+      <c r="V7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="C8" s="7" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
-        <v>6</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="10" t="s">
+      <c r="G8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="1">
+      <c r="H8" s="8"/>
+      <c r="I8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="1">
         <v>20</v>
       </c>
-      <c r="J8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="L8" s="1">
-        <v>1</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="N8" t="s">
-        <v>9</v>
+      <c r="K8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="O8" s="1">
         <v>1</v>
       </c>
-      <c r="P8" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="P8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q8" s="8"/>
+      <c r="R8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S8" s="1">
+        <v>1</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="U8" s="8"/>
+      <c r="V8" s="1">
+        <v>1</v>
+      </c>
+      <c r="W8" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="G9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="J9" s="1">
         <v>19</v>
       </c>
-      <c r="J9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="1">
-        <v>2</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>11</v>
+      <c r="K9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="O9" s="1">
         <v>2</v>
       </c>
-      <c r="P9" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="P9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="8"/>
+      <c r="S9" s="1">
+        <v>2</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="U9" s="8"/>
+      <c r="V9" s="1">
+        <v>2</v>
+      </c>
+      <c r="W9" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="1">
+      <c r="G10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="1">
         <v>18</v>
       </c>
-      <c r="J10" t="s">
-        <v>45</v>
-      </c>
-      <c r="L10" s="1">
-        <v>3</v>
+      <c r="K10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="M10" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="O10" s="1">
         <v>3</v>
       </c>
       <c r="P10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>54</v>
+      </c>
+      <c r="S10" s="1">
+        <v>3</v>
+      </c>
+      <c r="T10" t="s">
+        <v>15</v>
+      </c>
+      <c r="U10" t="s">
+        <v>66</v>
+      </c>
+      <c r="V10" s="1">
+        <v>3</v>
+      </c>
+      <c r="W10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D11" s="1">
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="1">
+      <c r="G11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="1">
         <v>17</v>
       </c>
-      <c r="J11" t="s">
-        <v>46</v>
-      </c>
-      <c r="L11" s="1">
-        <v>4</v>
+      <c r="K11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M11" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="O11" s="1">
         <v>4</v>
       </c>
       <c r="P11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>54</v>
+      </c>
+      <c r="S11" s="1">
+        <v>4</v>
+      </c>
+      <c r="T11" t="s">
+        <v>16</v>
+      </c>
+      <c r="V11" s="1">
+        <v>4</v>
+      </c>
+      <c r="W11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D12" s="1">
         <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="1">
+      <c r="G12" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="1">
         <v>16</v>
       </c>
-      <c r="J12" t="s">
-        <v>47</v>
-      </c>
-      <c r="L12" s="1">
-        <v>5</v>
+      <c r="K12" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="M12" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="O12" s="1">
         <v>5</v>
       </c>
       <c r="P12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>54</v>
+      </c>
+      <c r="S12" s="1">
+        <v>5</v>
+      </c>
+      <c r="T12" t="s">
+        <v>18</v>
+      </c>
+      <c r="U12" t="s">
+        <v>53</v>
+      </c>
+      <c r="V12" s="1">
+        <v>5</v>
+      </c>
+      <c r="W12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D13" s="1">
         <v>6</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="1">
+        <v>12</v>
+      </c>
+      <c r="J13" s="1">
         <v>15</v>
       </c>
-      <c r="J13" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" s="1">
-        <v>6</v>
+      <c r="K13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" t="s">
+        <v>13</v>
       </c>
       <c r="M13" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="O13" s="1">
         <v>6</v>
       </c>
       <c r="P13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="S13" s="1">
+        <v>6</v>
+      </c>
+      <c r="T13" t="s">
+        <v>51</v>
+      </c>
+      <c r="V13" s="1">
+        <v>6</v>
+      </c>
+      <c r="W13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D14" s="1">
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="1">
+      <c r="G14" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="1">
         <v>14</v>
       </c>
-      <c r="J14" t="s">
-        <v>12</v>
-      </c>
-      <c r="L14" s="1">
-        <v>7</v>
-      </c>
-      <c r="M14" t="s">
-        <v>24</v>
+      <c r="K14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="O14" s="1">
         <v>7</v>
       </c>
       <c r="P14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="S14" s="1">
+        <v>7</v>
+      </c>
+      <c r="T14" t="s">
+        <v>20</v>
+      </c>
+      <c r="V14" s="1">
+        <v>7</v>
+      </c>
+      <c r="W14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D15" s="1">
         <v>8</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="1">
+      <c r="G15" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="1">
         <v>13</v>
       </c>
-      <c r="J15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="1">
-        <v>8</v>
+      <c r="K15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="O15" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>52</v>
+      </c>
+      <c r="S15" s="1">
+        <v>8</v>
+      </c>
+      <c r="T15" t="s">
+        <v>52</v>
+      </c>
+      <c r="V15" s="1">
+        <v>8</v>
+      </c>
+      <c r="W15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D16" s="1">
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="1">
+        <v>21</v>
+      </c>
+      <c r="J16" s="1">
         <v>12</v>
       </c>
-      <c r="J16" t="s">
-        <v>19</v>
-      </c>
-      <c r="L16" s="1">
-        <v>9</v>
+      <c r="K16" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" t="s">
+        <v>21</v>
       </c>
       <c r="M16" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="O16" s="1">
         <v>9</v>
       </c>
       <c r="P16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="S16" s="1">
+        <v>9</v>
+      </c>
+      <c r="T16" t="s">
+        <v>23</v>
+      </c>
+      <c r="V16" s="1">
+        <v>9</v>
+      </c>
+      <c r="W16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D17" s="1">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="1">
+      <c r="G17" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="1">
         <v>11</v>
       </c>
-      <c r="J17" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="1">
-        <v>10</v>
-      </c>
-      <c r="M17" t="s">
-        <v>26</v>
+      <c r="K17" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="16" t="s">
+        <v>60</v>
       </c>
       <c r="O17" s="1">
         <v>10</v>
       </c>
       <c r="P17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="4:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="S17" s="1">
+        <v>10</v>
+      </c>
+      <c r="T17" t="s">
+        <v>22</v>
+      </c>
+      <c r="V17" s="1">
+        <v>10</v>
+      </c>
+      <c r="W17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="G18" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="1">
+      <c r="G18" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="1">
         <v>10</v>
       </c>
-      <c r="J18" t="s">
-        <v>22</v>
-      </c>
-      <c r="L18" s="1">
-        <v>11</v>
-      </c>
-      <c r="M18" t="s">
-        <v>28</v>
+      <c r="K18" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="O18" s="1">
         <v>11</v>
       </c>
-      <c r="P18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="P18" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q18" s="12"/>
+      <c r="S18" s="1">
+        <v>11</v>
+      </c>
+      <c r="T18" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="U18" s="12"/>
+      <c r="V18" s="1">
+        <v>11</v>
+      </c>
+      <c r="W18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <v>12</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I19" s="1">
+        <v>67</v>
+      </c>
+      <c r="J19" s="1">
         <v>9</v>
       </c>
-      <c r="J19" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" s="1">
-        <v>12</v>
-      </c>
-      <c r="M19" s="12" t="s">
-        <v>29</v>
+      <c r="K19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M19" t="s">
+        <v>58</v>
       </c>
       <c r="O19" s="1">
         <v>12</v>
       </c>
-      <c r="P19" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="P19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q19" s="9"/>
+      <c r="S19" s="1">
+        <v>12</v>
+      </c>
+      <c r="T19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="U19" s="9"/>
+      <c r="V19" s="1">
+        <v>12</v>
+      </c>
+      <c r="W19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20" s="1">
+      <c r="G20" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="1">
         <v>8</v>
       </c>
-      <c r="J20" t="s">
-        <v>24</v>
-      </c>
-      <c r="O20" s="1">
+      <c r="K20" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" t="s">
+        <v>70</v>
+      </c>
+      <c r="S20" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="V20" s="1">
+        <v>13</v>
+      </c>
+      <c r="W20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F21" s="1"/>
-      <c r="G21" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21" s="1">
+      <c r="G21" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" t="s">
+        <v>45</v>
+      </c>
+      <c r="J21" s="1">
         <v>7</v>
       </c>
-      <c r="J21" t="s">
-        <v>25</v>
-      </c>
-      <c r="O21" s="1">
+      <c r="K21" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="M21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S21" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="V21" s="1">
+        <v>14</v>
+      </c>
+      <c r="W21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <v>15</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" t="s">
-        <v>26</v>
-      </c>
-      <c r="I22" s="1">
+      <c r="G22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" t="s">
+        <v>45</v>
+      </c>
+      <c r="J22" s="1">
         <v>6</v>
       </c>
-      <c r="J22" t="s">
-        <v>26</v>
-      </c>
-      <c r="O22" s="1">
+      <c r="K22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="S22" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="V22" s="1">
+        <v>15</v>
+      </c>
+      <c r="W22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I23" s="1">
+      <c r="G23" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" t="s">
+        <v>45</v>
+      </c>
+      <c r="J23" s="1">
         <v>5</v>
       </c>
-      <c r="J23" t="s">
-        <v>27</v>
-      </c>
-      <c r="O23" s="1">
+      <c r="K23" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L23" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="S23" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="V23" s="1">
+        <v>16</v>
+      </c>
+      <c r="W23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D24" s="1">
         <v>17</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="1"/>
+      <c r="E24" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G24" t="s">
-        <v>20</v>
-      </c>
-      <c r="I24" s="1">
+        <v>16</v>
+      </c>
+      <c r="J24" s="1">
         <v>4</v>
       </c>
-      <c r="J24" t="s">
-        <v>20</v>
-      </c>
-      <c r="O24" s="1">
+      <c r="K24" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" t="s">
+        <v>16</v>
+      </c>
+      <c r="M24" t="s">
+        <v>59</v>
+      </c>
+      <c r="S24" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="V24" s="1">
+        <v>17</v>
+      </c>
+      <c r="W24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D25" s="1">
         <v>18</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="1">
+      <c r="G25" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="J25" s="1">
         <v>3</v>
       </c>
-      <c r="J25" t="s">
-        <v>28</v>
-      </c>
-      <c r="O25" s="1">
+      <c r="K25" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="S25" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="V25" s="1">
+        <v>18</v>
+      </c>
+      <c r="W25" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D26" s="1">
         <v>19</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="I26" s="1">
+      <c r="G26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="9"/>
+      <c r="J26" s="1">
         <v>2</v>
       </c>
-      <c r="J26" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="O26" s="1">
+      <c r="K26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="S26" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="V26" s="1">
+        <v>19</v>
+      </c>
+      <c r="W26" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
         <v>20</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="I27" s="1">
+      <c r="G27" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" s="9"/>
+      <c r="J27" s="1">
         <v>1</v>
       </c>
-      <c r="J27" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="O27" s="1">
+      <c r="K27" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="S27" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-    </row>
-    <row r="29" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-    </row>
-    <row r="31" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="E31" s="13"/>
+      <c r="V27" s="1">
+        <v>20</v>
+      </c>
+      <c r="W27" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="W28" s="1"/>
+    </row>
+    <row r="29" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+    </row>
+    <row r="31" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="E31" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C3:Q3"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="C3:V3"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="V6:X6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
TP Location for debug
</commit_message>
<xml_diff>
--- a/Hardware Inteconnects.xlsx
+++ b/Hardware Inteconnects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kashi\OneDrive - Airzai\Airzai\GitHub\PCB Design\Airzai-PCB-Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kashif\OneDrive - Airzai\Airzai\GitHub\Airzai-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="6_{9706E25E-717C-4DF6-87EF-534170850AE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{BD6E8713-6316-4695-91AC-E575F64590AD}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="114_{36E60E0A-9DA8-40D6-9B9D-D42CFEE01F4A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{D12C5934-ABF2-49B8-B11B-18C572B75B68}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="30915" windowHeight="15796" xr2:uid="{BDE72F7E-F162-48FD-B3AC-A08C53C45481}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BDE72F7E-F162-48FD-B3AC-A08C53C45481}"/>
   </bookViews>
   <sheets>
     <sheet name="Airzai Interconnects" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="97">
   <si>
     <t>Pin Number</t>
   </si>
@@ -238,6 +238,90 @@
   </si>
   <si>
     <t>SW1 GPIO</t>
+  </si>
+  <si>
+    <t>TP6</t>
+  </si>
+  <si>
+    <t>TP7</t>
+  </si>
+  <si>
+    <t>TP8</t>
+  </si>
+  <si>
+    <t>TP9</t>
+  </si>
+  <si>
+    <t>TP10</t>
+  </si>
+  <si>
+    <t>TP11</t>
+  </si>
+  <si>
+    <t>TP12</t>
+  </si>
+  <si>
+    <t>TP13</t>
+  </si>
+  <si>
+    <t>TP14</t>
+  </si>
+  <si>
+    <t>TP15</t>
+  </si>
+  <si>
+    <t>TP16</t>
+  </si>
+  <si>
+    <t>TP17</t>
+  </si>
+  <si>
+    <t>TP18</t>
+  </si>
+  <si>
+    <t>TP19</t>
+  </si>
+  <si>
+    <t>TP20</t>
+  </si>
+  <si>
+    <t>TP21</t>
+  </si>
+  <si>
+    <t>TP22</t>
+  </si>
+  <si>
+    <t>VCC_5V_USB</t>
+  </si>
+  <si>
+    <t>VCC_3V_Reg</t>
+  </si>
+  <si>
+    <t>VCC_3V_J14</t>
+  </si>
+  <si>
+    <t>VCC_5V_J14</t>
+  </si>
+  <si>
+    <t>EN_Line</t>
+  </si>
+  <si>
+    <t>LED_STR_Data</t>
+  </si>
+  <si>
+    <t>LED_STR_CLK</t>
+  </si>
+  <si>
+    <t>TP23</t>
+  </si>
+  <si>
+    <t>TOF_INT</t>
+  </si>
+  <si>
+    <t>NFC_INT</t>
+  </si>
+  <si>
+    <t>ACCL_INT</t>
   </si>
 </sst>
 </file>
@@ -743,40 +827,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC17FFE-34FD-4EEC-ACA2-98BFA418FDBF}">
-  <dimension ref="C2:X31"/>
+  <dimension ref="C2:X54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="7" max="7" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.59765625" customWidth="1"/>
-    <col min="9" max="9" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.59765625" customWidth="1"/>
-    <col min="12" max="12" width="21.86328125" customWidth="1"/>
-    <col min="13" max="13" width="27.73046875" customWidth="1"/>
-    <col min="14" max="14" width="21.73046875" customWidth="1"/>
-    <col min="15" max="15" width="11.59765625" customWidth="1"/>
-    <col min="16" max="16" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.73046875" customWidth="1"/>
-    <col min="18" max="18" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.73046875" customWidth="1"/>
-    <col min="21" max="21" width="11.59765625" customWidth="1"/>
-    <col min="22" max="22" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:24" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="3:24" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="20" t="s">
         <v>49</v>
       </c>
@@ -801,7 +885,7 @@
       <c r="V3" s="22"/>
       <c r="W3" s="2"/>
     </row>
-    <row r="6" spans="3:24" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C6" s="19" t="s">
         <v>47</v>
       </c>
@@ -833,7 +917,7 @@
       <c r="W6" s="24"/>
       <c r="X6" s="24"/>
     </row>
-    <row r="7" spans="3:24" x14ac:dyDescent="0.45">
+    <row r="7" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>6</v>
       </c>
@@ -898,7 +982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="3:24" x14ac:dyDescent="0.45">
+    <row r="8" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
@@ -951,7 +1035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="3:24" x14ac:dyDescent="0.45">
+    <row r="9" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
         <v>2</v>
       </c>
@@ -991,7 +1075,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="3:24" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
         <v>3</v>
       </c>
@@ -1039,7 +1123,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="3:24" x14ac:dyDescent="0.45">
+    <row r="11" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D11" s="1">
         <v>4</v>
       </c>
@@ -1084,7 +1168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="3:24" x14ac:dyDescent="0.45">
+    <row r="12" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D12" s="1">
         <v>5</v>
       </c>
@@ -1132,7 +1216,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="3:24" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D13" s="1">
         <v>6</v>
       </c>
@@ -1174,7 +1258,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="3:24" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D14" s="1">
         <v>7</v>
       </c>
@@ -1213,7 +1297,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="3:24" x14ac:dyDescent="0.45">
+    <row r="15" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D15" s="1">
         <v>8</v>
       </c>
@@ -1252,7 +1336,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="3:24" x14ac:dyDescent="0.45">
+    <row r="16" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D16" s="1">
         <v>9</v>
       </c>
@@ -1294,7 +1378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D17" s="1">
         <v>10</v>
       </c>
@@ -1333,7 +1417,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <v>11</v>
       </c>
@@ -1374,7 +1458,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <v>12</v>
       </c>
@@ -1418,7 +1502,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <v>13</v>
       </c>
@@ -1448,7 +1532,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <v>14</v>
       </c>
@@ -1484,7 +1568,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <v>15</v>
       </c>
@@ -1517,7 +1601,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <v>16</v>
       </c>
@@ -1550,7 +1634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D24" s="1">
         <v>17</v>
       </c>
@@ -1585,7 +1669,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D25" s="1">
         <v>18</v>
       </c>
@@ -1614,7 +1698,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D26" s="1">
         <v>19</v>
       </c>
@@ -1648,7 +1732,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
         <v>20</v>
       </c>
@@ -1682,7 +1766,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:23" x14ac:dyDescent="0.25">
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
@@ -1690,15 +1774,169 @@
       <c r="Q28" s="10"/>
       <c r="W28" s="1"/>
     </row>
-    <row r="29" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:23" x14ac:dyDescent="0.25">
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
     </row>
-    <row r="31" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:23" x14ac:dyDescent="0.25">
       <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>75</v>
+      </c>
+      <c r="E38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>79</v>
+      </c>
+      <c r="E42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
updated NFC Reader Project
</commit_message>
<xml_diff>
--- a/Hardware Inteconnects.xlsx
+++ b/Hardware Inteconnects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kashif\OneDrive - Airzai\Airzai\GitHub\Airzai-Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kashif\OneDrive - Airzai\Airzai\GitHub\PCB Design\Airzai-PCB-Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="114_{36E60E0A-9DA8-40D6-9B9D-D42CFEE01F4A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{D12C5934-ABF2-49B8-B11B-18C572B75B68}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="6_{9706E25E-717C-4DF6-87EF-534170850AE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B7E4B585-F5AB-4320-A5F5-EA36946546D2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BDE72F7E-F162-48FD-B3AC-A08C53C45481}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="69">
   <si>
     <t>Pin Number</t>
   </si>
@@ -141,9 +141,6 @@
     <t>P50_GPIO_00</t>
   </si>
   <si>
-    <t>P55_GPIO_01</t>
-  </si>
-  <si>
     <t>P57_GPIO_02</t>
   </si>
   <si>
@@ -240,88 +237,7 @@
     <t>SW1 GPIO</t>
   </si>
   <si>
-    <t>TP6</t>
-  </si>
-  <si>
-    <t>TP7</t>
-  </si>
-  <si>
-    <t>TP8</t>
-  </si>
-  <si>
-    <t>TP9</t>
-  </si>
-  <si>
-    <t>TP10</t>
-  </si>
-  <si>
-    <t>TP11</t>
-  </si>
-  <si>
-    <t>TP12</t>
-  </si>
-  <si>
-    <t>TP13</t>
-  </si>
-  <si>
-    <t>TP14</t>
-  </si>
-  <si>
-    <t>TP15</t>
-  </si>
-  <si>
-    <t>TP16</t>
-  </si>
-  <si>
-    <t>TP17</t>
-  </si>
-  <si>
-    <t>TP18</t>
-  </si>
-  <si>
-    <t>TP19</t>
-  </si>
-  <si>
-    <t>TP20</t>
-  </si>
-  <si>
-    <t>TP21</t>
-  </si>
-  <si>
-    <t>TP22</t>
-  </si>
-  <si>
-    <t>VCC_5V_USB</t>
-  </si>
-  <si>
-    <t>VCC_3V_Reg</t>
-  </si>
-  <si>
-    <t>VCC_3V_J14</t>
-  </si>
-  <si>
-    <t>VCC_5V_J14</t>
-  </si>
-  <si>
-    <t>EN_Line</t>
-  </si>
-  <si>
-    <t>LED_STR_Data</t>
-  </si>
-  <si>
-    <t>LED_STR_CLK</t>
-  </si>
-  <si>
-    <t>TP23</t>
-  </si>
-  <si>
-    <t>TOF_INT</t>
-  </si>
-  <si>
-    <t>NFC_INT</t>
-  </si>
-  <si>
-    <t>ACCL_INT</t>
+    <t>P55_GPIO_28</t>
   </si>
 </sst>
 </file>
@@ -827,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC17FFE-34FD-4EEC-ACA2-98BFA418FDBF}">
-  <dimension ref="C2:X54"/>
+  <dimension ref="C2:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,7 +778,7 @@
     <row r="2" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
@@ -887,7 +803,7 @@
     </row>
     <row r="6" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C6" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
@@ -895,7 +811,7 @@
       <c r="G6" s="19"/>
       <c r="H6" s="4"/>
       <c r="I6" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J6" s="23"/>
       <c r="K6" s="23"/>
@@ -906,13 +822,13 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S6" s="19"/>
       <c r="T6" s="19"/>
       <c r="U6" s="6"/>
       <c r="V6" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="W6" s="24"/>
       <c r="X6" s="24"/>
@@ -943,10 +859,10 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" t="s">
         <v>55</v>
-      </c>
-      <c r="L7" t="s">
-        <v>56</v>
       </c>
       <c r="M7" t="s">
         <v>2</v>
@@ -1009,7 +925,7 @@
       </c>
       <c r="M8" s="7"/>
       <c r="N8" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O8" s="1">
         <v>1</v>
@@ -1080,20 +996,20 @@
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="14" t="s">
         <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J10" s="1">
         <v>18</v>
       </c>
       <c r="K10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L10" s="14" t="s">
         <v>8</v>
@@ -1105,7 +1021,7 @@
         <v>15</v>
       </c>
       <c r="Q10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S10" s="1">
         <v>3</v>
@@ -1114,7 +1030,7 @@
         <v>15</v>
       </c>
       <c r="U10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V10" s="1">
         <v>3</v>
@@ -1128,20 +1044,20 @@
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="14" t="s">
         <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J11" s="1">
         <v>17</v>
       </c>
       <c r="K11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L11" s="14" t="s">
         <v>10</v>
@@ -1153,7 +1069,7 @@
         <v>16</v>
       </c>
       <c r="Q11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S11" s="1">
         <v>4</v>
@@ -1173,7 +1089,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="18" t="s">
@@ -1183,13 +1099,13 @@
         <v>16</v>
       </c>
       <c r="K12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="M12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O12" s="1">
         <v>5</v>
@@ -1198,7 +1114,7 @@
         <v>18</v>
       </c>
       <c r="Q12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S12" s="1">
         <v>5</v>
@@ -1207,7 +1123,7 @@
         <v>18</v>
       </c>
       <c r="U12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V12" s="1">
         <v>5</v>
@@ -1221,12 +1137,13 @@
         <v>6</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" t="s">
         <v>12</v>
       </c>
+      <c r="H13" s="18"/>
       <c r="J13" s="1">
         <v>15</v>
       </c>
@@ -1237,19 +1154,19 @@
         <v>13</v>
       </c>
       <c r="M13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O13" s="1">
         <v>6</v>
       </c>
       <c r="P13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S13" s="1">
         <v>6</v>
       </c>
       <c r="T13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V13" s="1">
         <v>6</v>
@@ -1263,12 +1180,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="18" t="s">
         <v>13</v>
       </c>
+      <c r="H14" t="s">
+        <v>51</v>
+      </c>
       <c r="J14" s="1">
         <v>14</v>
       </c>
@@ -1276,7 +1196,7 @@
         <v>8</v>
       </c>
       <c r="L14" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O14" s="1">
         <v>7</v>
@@ -1308,6 +1228,9 @@
       <c r="G15" s="18" t="s">
         <v>14</v>
       </c>
+      <c r="H15" t="s">
+        <v>50</v>
+      </c>
       <c r="J15" s="1">
         <v>13</v>
       </c>
@@ -1315,19 +1238,19 @@
         <v>10</v>
       </c>
       <c r="L15" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O15" s="1">
         <v>8</v>
       </c>
       <c r="P15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="S15" s="1">
         <v>8</v>
       </c>
       <c r="T15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V15" s="1">
         <v>8</v>
@@ -1354,10 +1277,10 @@
         <v>15</v>
       </c>
       <c r="L16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O16" s="1">
         <v>9</v>
@@ -1378,7 +1301,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D17" s="1">
         <v>10</v>
       </c>
@@ -1387,7 +1310,7 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J17" s="1">
         <v>11</v>
@@ -1396,7 +1319,7 @@
         <v>16</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O17" s="1">
         <v>10</v>
@@ -1417,7 +1340,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <v>11</v>
       </c>
@@ -1426,7 +1349,7 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J18" s="1">
         <v>10</v>
@@ -1435,7 +1358,7 @@
         <v>18</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O18" s="1">
         <v>11</v>
@@ -1458,7 +1381,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <v>12</v>
       </c>
@@ -1467,7 +1390,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J19" s="1">
         <v>9</v>
@@ -1476,10 +1399,10 @@
         <v>19</v>
       </c>
       <c r="L19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O19" s="1">
         <v>12</v>
@@ -1502,7 +1425,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <v>13</v>
       </c>
@@ -1532,7 +1455,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <v>14</v>
       </c>
@@ -1541,10 +1464,10 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J21" s="1">
         <v>7</v>
@@ -1553,10 +1476,10 @@
         <v>21</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S21" s="1">
         <v>14</v>
@@ -1568,7 +1491,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <v>15</v>
       </c>
@@ -1580,7 +1503,7 @@
         <v>22</v>
       </c>
       <c r="H22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J22" s="1">
         <v>6</v>
@@ -1601,7 +1524,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <v>16</v>
       </c>
@@ -1613,7 +1536,7 @@
         <v>23</v>
       </c>
       <c r="H23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J23" s="1">
         <v>5</v>
@@ -1634,15 +1557,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D24" s="1">
         <v>17</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G24" t="s">
         <v>16</v>
@@ -1657,7 +1580,7 @@
         <v>16</v>
       </c>
       <c r="M24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S24" s="1">
         <v>17</v>
@@ -1669,7 +1592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D25" s="1">
         <v>18</v>
       </c>
@@ -1698,7 +1621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D26" s="1">
         <v>19</v>
       </c>
@@ -1732,7 +1655,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
         <v>20</v>
       </c>
@@ -1766,7 +1689,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:23" x14ac:dyDescent="0.25">
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
@@ -1774,169 +1697,15 @@
       <c r="Q28" s="10"/>
       <c r="W28" s="1"/>
     </row>
-    <row r="29" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:23" x14ac:dyDescent="0.25">
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
     </row>
-    <row r="31" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:23" x14ac:dyDescent="0.25">
       <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>71</v>
-      </c>
-      <c r="E34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>74</v>
-      </c>
-      <c r="E37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>75</v>
-      </c>
-      <c r="E38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>76</v>
-      </c>
-      <c r="E39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>77</v>
-      </c>
-      <c r="E40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>79</v>
-      </c>
-      <c r="E42" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>80</v>
-      </c>
-      <c r="E43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>81</v>
-      </c>
-      <c r="E44" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>82</v>
-      </c>
-      <c r="E45" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>85</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>